<commit_message>
Updated Exam Center code Changes
</commit_message>
<xml_diff>
--- a/src/test/resources/Files/ControllerTemplate.xlsx
+++ b/src/test/resources/Files/ControllerTemplate.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1365" uniqueCount="1365">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1965" uniqueCount="1961">
   <si>
     <t>FirstName</t>
   </si>
@@ -4120,6 +4120,1794 @@
   </si>
   <si>
     <t>02509</t>
+  </si>
+  <si>
+    <t>Controller70439</t>
+  </si>
+  <si>
+    <t>Automation70439</t>
+  </si>
+  <si>
+    <t>controllerautomation70439@gmail.com</t>
+  </si>
+  <si>
+    <t>70439</t>
+  </si>
+  <si>
+    <t>Controller61515</t>
+  </si>
+  <si>
+    <t>Automation61515</t>
+  </si>
+  <si>
+    <t>controllerautomation61515@gmail.com</t>
+  </si>
+  <si>
+    <t>61515</t>
+  </si>
+  <si>
+    <t>Controller88964</t>
+  </si>
+  <si>
+    <t>Automation88964</t>
+  </si>
+  <si>
+    <t>controllerautomation88964@gmail.com</t>
+  </si>
+  <si>
+    <t>88964</t>
+  </si>
+  <si>
+    <t>Controller19034</t>
+  </si>
+  <si>
+    <t>Automation19034</t>
+  </si>
+  <si>
+    <t>controllerautomation19034@gmail.com</t>
+  </si>
+  <si>
+    <t>19034</t>
+  </si>
+  <si>
+    <t>Controller74275</t>
+  </si>
+  <si>
+    <t>Automation74275</t>
+  </si>
+  <si>
+    <t>controllerautomation74275@gmail.com</t>
+  </si>
+  <si>
+    <t>74275</t>
+  </si>
+  <si>
+    <t>Controller72554</t>
+  </si>
+  <si>
+    <t>Automation72554</t>
+  </si>
+  <si>
+    <t>controllerautomation72554@gmail.com</t>
+  </si>
+  <si>
+    <t>72554</t>
+  </si>
+  <si>
+    <t>Controller11840</t>
+  </si>
+  <si>
+    <t>Automation11840</t>
+  </si>
+  <si>
+    <t>controllerautomation11840@gmail.com</t>
+  </si>
+  <si>
+    <t>11840</t>
+  </si>
+  <si>
+    <t>Controller26332</t>
+  </si>
+  <si>
+    <t>Automation26332</t>
+  </si>
+  <si>
+    <t>controllerautomation26332@gmail.com</t>
+  </si>
+  <si>
+    <t>26332</t>
+  </si>
+  <si>
+    <t>Controller31358</t>
+  </si>
+  <si>
+    <t>Automation31358</t>
+  </si>
+  <si>
+    <t>controllerautomation31358@gmail.com</t>
+  </si>
+  <si>
+    <t>31358</t>
+  </si>
+  <si>
+    <t>Controller89440</t>
+  </si>
+  <si>
+    <t>Automation89440</t>
+  </si>
+  <si>
+    <t>controllerautomation89440@gmail.com</t>
+  </si>
+  <si>
+    <t>89440</t>
+  </si>
+  <si>
+    <t>Controller62430</t>
+  </si>
+  <si>
+    <t>Automation62430</t>
+  </si>
+  <si>
+    <t>controllerautomation62430@gmail.com</t>
+  </si>
+  <si>
+    <t>62430</t>
+  </si>
+  <si>
+    <t>Controller33727</t>
+  </si>
+  <si>
+    <t>Automation33727</t>
+  </si>
+  <si>
+    <t>controllerautomation33727@gmail.com</t>
+  </si>
+  <si>
+    <t>33727</t>
+  </si>
+  <si>
+    <t>Controller54897</t>
+  </si>
+  <si>
+    <t>Automation54897</t>
+  </si>
+  <si>
+    <t>controllerautomation54897@gmail.com</t>
+  </si>
+  <si>
+    <t>54897</t>
+  </si>
+  <si>
+    <t>Controller60073</t>
+  </si>
+  <si>
+    <t>Automation60073</t>
+  </si>
+  <si>
+    <t>controllerautomation60073@gmail.com</t>
+  </si>
+  <si>
+    <t>60073</t>
+  </si>
+  <si>
+    <t>Controller34855</t>
+  </si>
+  <si>
+    <t>Automation34855</t>
+  </si>
+  <si>
+    <t>controllerautomation34855@gmail.com</t>
+  </si>
+  <si>
+    <t>34855</t>
+  </si>
+  <si>
+    <t>Controller41840</t>
+  </si>
+  <si>
+    <t>Automation41840</t>
+  </si>
+  <si>
+    <t>controllerautomation41840@gmail.com</t>
+  </si>
+  <si>
+    <t>41840</t>
+  </si>
+  <si>
+    <t>Controller76190</t>
+  </si>
+  <si>
+    <t>Automation76190</t>
+  </si>
+  <si>
+    <t>controllerautomation76190@gmail.com</t>
+  </si>
+  <si>
+    <t>76190</t>
+  </si>
+  <si>
+    <t>Controller83491</t>
+  </si>
+  <si>
+    <t>Automation83491</t>
+  </si>
+  <si>
+    <t>controllerautomation83491@gmail.com</t>
+  </si>
+  <si>
+    <t>83491</t>
+  </si>
+  <si>
+    <t>Controller19839</t>
+  </si>
+  <si>
+    <t>Automation19839</t>
+  </si>
+  <si>
+    <t>controllerautomation19839@gmail.com</t>
+  </si>
+  <si>
+    <t>19839</t>
+  </si>
+  <si>
+    <t>Controller52267</t>
+  </si>
+  <si>
+    <t>Automation52267</t>
+  </si>
+  <si>
+    <t>controllerautomation52267@gmail.com</t>
+  </si>
+  <si>
+    <t>52267</t>
+  </si>
+  <si>
+    <t>Controller79851</t>
+  </si>
+  <si>
+    <t>Automation79851</t>
+  </si>
+  <si>
+    <t>controllerautomation79851@gmail.com</t>
+  </si>
+  <si>
+    <t>79851</t>
+  </si>
+  <si>
+    <t>Controller26394</t>
+  </si>
+  <si>
+    <t>Automation26394</t>
+  </si>
+  <si>
+    <t>controllerautomation26394@gmail.com</t>
+  </si>
+  <si>
+    <t>26394</t>
+  </si>
+  <si>
+    <t>Controller09500</t>
+  </si>
+  <si>
+    <t>Automation09500</t>
+  </si>
+  <si>
+    <t>controllerautomation09500@gmail.com</t>
+  </si>
+  <si>
+    <t>09500</t>
+  </si>
+  <si>
+    <t>Controller57191</t>
+  </si>
+  <si>
+    <t>Automation57191</t>
+  </si>
+  <si>
+    <t>controllerautomation57191@gmail.com</t>
+  </si>
+  <si>
+    <t>57191</t>
+  </si>
+  <si>
+    <t>Controller09483</t>
+  </si>
+  <si>
+    <t>Automation09483</t>
+  </si>
+  <si>
+    <t>controllerautomation09483@gmail.com</t>
+  </si>
+  <si>
+    <t>09483</t>
+  </si>
+  <si>
+    <t>Controller41430</t>
+  </si>
+  <si>
+    <t>Automation41430</t>
+  </si>
+  <si>
+    <t>controllerautomation41430@gmail.com</t>
+  </si>
+  <si>
+    <t>41430</t>
+  </si>
+  <si>
+    <t>Controller00397</t>
+  </si>
+  <si>
+    <t>Automation00397</t>
+  </si>
+  <si>
+    <t>controllerautomation00397@gmail.com</t>
+  </si>
+  <si>
+    <t>00397</t>
+  </si>
+  <si>
+    <t>Controller83285</t>
+  </si>
+  <si>
+    <t>Automation83285</t>
+  </si>
+  <si>
+    <t>controllerautomation83285@gmail.com</t>
+  </si>
+  <si>
+    <t>83285</t>
+  </si>
+  <si>
+    <t>Controller44257</t>
+  </si>
+  <si>
+    <t>Automation44257</t>
+  </si>
+  <si>
+    <t>controllerautomation44257@gmail.com</t>
+  </si>
+  <si>
+    <t>44257</t>
+  </si>
+  <si>
+    <t>Controller09962</t>
+  </si>
+  <si>
+    <t>Automation09962</t>
+  </si>
+  <si>
+    <t>controllerautomation09962@gmail.com</t>
+  </si>
+  <si>
+    <t>09962</t>
+  </si>
+  <si>
+    <t>Controller00740</t>
+  </si>
+  <si>
+    <t>Automation00740</t>
+  </si>
+  <si>
+    <t>controllerautomation00740@gmail.com</t>
+  </si>
+  <si>
+    <t>00740</t>
+  </si>
+  <si>
+    <t>Controller74030</t>
+  </si>
+  <si>
+    <t>Automation74030</t>
+  </si>
+  <si>
+    <t>controllerautomation74030@gmail.com</t>
+  </si>
+  <si>
+    <t>74030</t>
+  </si>
+  <si>
+    <t>Controller31115</t>
+  </si>
+  <si>
+    <t>Automation31115</t>
+  </si>
+  <si>
+    <t>controllerautomation31115@gmail.com</t>
+  </si>
+  <si>
+    <t>31115</t>
+  </si>
+  <si>
+    <t>Controller43945</t>
+  </si>
+  <si>
+    <t>Automation43945</t>
+  </si>
+  <si>
+    <t>controllerautomation43945@gmail.com</t>
+  </si>
+  <si>
+    <t>43945</t>
+  </si>
+  <si>
+    <t>Controller05514</t>
+  </si>
+  <si>
+    <t>Automation05514</t>
+  </si>
+  <si>
+    <t>controllerautomation05514@gmail.com</t>
+  </si>
+  <si>
+    <t>05514</t>
+  </si>
+  <si>
+    <t>Controller86705</t>
+  </si>
+  <si>
+    <t>Automation86705</t>
+  </si>
+  <si>
+    <t>controllerautomation86705@gmail.com</t>
+  </si>
+  <si>
+    <t>86705</t>
+  </si>
+  <si>
+    <t>Controller96031</t>
+  </si>
+  <si>
+    <t>Automation96031</t>
+  </si>
+  <si>
+    <t>controllerautomation96031@gmail.com</t>
+  </si>
+  <si>
+    <t>96031</t>
+  </si>
+  <si>
+    <t>Controller16231</t>
+  </si>
+  <si>
+    <t>Automation16231</t>
+  </si>
+  <si>
+    <t>controllerautomation16231@gmail.com</t>
+  </si>
+  <si>
+    <t>16231</t>
+  </si>
+  <si>
+    <t>Controller06377</t>
+  </si>
+  <si>
+    <t>Automation06377</t>
+  </si>
+  <si>
+    <t>controllerautomation06377@gmail.com</t>
+  </si>
+  <si>
+    <t>06377</t>
+  </si>
+  <si>
+    <t>Controller43548</t>
+  </si>
+  <si>
+    <t>Automation43548</t>
+  </si>
+  <si>
+    <t>controllerautomation43548@gmail.com</t>
+  </si>
+  <si>
+    <t>43548</t>
+  </si>
+  <si>
+    <t>Controller50895</t>
+  </si>
+  <si>
+    <t>Automation50895</t>
+  </si>
+  <si>
+    <t>controllerautomation50895@gmail.com</t>
+  </si>
+  <si>
+    <t>50895</t>
+  </si>
+  <si>
+    <t>Controller28337</t>
+  </si>
+  <si>
+    <t>Automation28337</t>
+  </si>
+  <si>
+    <t>controllerautomation28337@gmail.com</t>
+  </si>
+  <si>
+    <t>28337</t>
+  </si>
+  <si>
+    <t>Controller85444</t>
+  </si>
+  <si>
+    <t>Automation85444</t>
+  </si>
+  <si>
+    <t>controllerautomation85444@gmail.com</t>
+  </si>
+  <si>
+    <t>85444</t>
+  </si>
+  <si>
+    <t>Controller32161</t>
+  </si>
+  <si>
+    <t>Automation32161</t>
+  </si>
+  <si>
+    <t>controllerautomation32161@gmail.com</t>
+  </si>
+  <si>
+    <t>32161</t>
+  </si>
+  <si>
+    <t>Controller83823</t>
+  </si>
+  <si>
+    <t>Automation83823</t>
+  </si>
+  <si>
+    <t>controllerautomation83823@gmail.com</t>
+  </si>
+  <si>
+    <t>83823</t>
+  </si>
+  <si>
+    <t>Controller05526</t>
+  </si>
+  <si>
+    <t>Automation05526</t>
+  </si>
+  <si>
+    <t>controllerautomation05526@gmail.com</t>
+  </si>
+  <si>
+    <t>05526</t>
+  </si>
+  <si>
+    <t>Controller76064</t>
+  </si>
+  <si>
+    <t>Automation76064</t>
+  </si>
+  <si>
+    <t>controllerautomation76064@gmail.com</t>
+  </si>
+  <si>
+    <t>76064</t>
+  </si>
+  <si>
+    <t>Controller76999</t>
+  </si>
+  <si>
+    <t>Automation76999</t>
+  </si>
+  <si>
+    <t>controllerautomation76999@gmail.com</t>
+  </si>
+  <si>
+    <t>76999</t>
+  </si>
+  <si>
+    <t>Controller89654</t>
+  </si>
+  <si>
+    <t>Automation89654</t>
+  </si>
+  <si>
+    <t>controllerautomation89654@gmail.com</t>
+  </si>
+  <si>
+    <t>89654</t>
+  </si>
+  <si>
+    <t>Controller84374</t>
+  </si>
+  <si>
+    <t>Automation84374</t>
+  </si>
+  <si>
+    <t>controllerautomation84374@gmail.com</t>
+  </si>
+  <si>
+    <t>84374</t>
+  </si>
+  <si>
+    <t>Controller45801</t>
+  </si>
+  <si>
+    <t>Automation45801</t>
+  </si>
+  <si>
+    <t>controllerautomation45801@gmail.com</t>
+  </si>
+  <si>
+    <t>45801</t>
+  </si>
+  <si>
+    <t>Controller54856</t>
+  </si>
+  <si>
+    <t>Automation54856</t>
+  </si>
+  <si>
+    <t>controllerautomation54856@gmail.com</t>
+  </si>
+  <si>
+    <t>54856</t>
+  </si>
+  <si>
+    <t>Controller69181</t>
+  </si>
+  <si>
+    <t>Automation69181</t>
+  </si>
+  <si>
+    <t>controllerautomation69181@gmail.com</t>
+  </si>
+  <si>
+    <t>69181</t>
+  </si>
+  <si>
+    <t>Controller04230</t>
+  </si>
+  <si>
+    <t>Automation04230</t>
+  </si>
+  <si>
+    <t>controllerautomation04230@gmail.com</t>
+  </si>
+  <si>
+    <t>04230</t>
+  </si>
+  <si>
+    <t>Controller73705</t>
+  </si>
+  <si>
+    <t>Automation73705</t>
+  </si>
+  <si>
+    <t>controllerautomation73705@gmail.com</t>
+  </si>
+  <si>
+    <t>73705</t>
+  </si>
+  <si>
+    <t>Controller90378</t>
+  </si>
+  <si>
+    <t>Automation90378</t>
+  </si>
+  <si>
+    <t>controllerautomation90378@gmail.com</t>
+  </si>
+  <si>
+    <t>90378</t>
+  </si>
+  <si>
+    <t>Controller68714</t>
+  </si>
+  <si>
+    <t>Automation68714</t>
+  </si>
+  <si>
+    <t>controllerautomation68714@gmail.com</t>
+  </si>
+  <si>
+    <t>68714</t>
+  </si>
+  <si>
+    <t>Controller36458</t>
+  </si>
+  <si>
+    <t>Automation36458</t>
+  </si>
+  <si>
+    <t>controllerautomation36458@gmail.com</t>
+  </si>
+  <si>
+    <t>36458</t>
+  </si>
+  <si>
+    <t>Controller64891</t>
+  </si>
+  <si>
+    <t>Automation64891</t>
+  </si>
+  <si>
+    <t>controllerautomation64891@gmail.com</t>
+  </si>
+  <si>
+    <t>64891</t>
+  </si>
+  <si>
+    <t>Controller24319</t>
+  </si>
+  <si>
+    <t>Automation24319</t>
+  </si>
+  <si>
+    <t>controllerautomation24319@gmail.com</t>
+  </si>
+  <si>
+    <t>24319</t>
+  </si>
+  <si>
+    <t>Controller48632</t>
+  </si>
+  <si>
+    <t>Automation48632</t>
+  </si>
+  <si>
+    <t>controllerautomation48632@gmail.com</t>
+  </si>
+  <si>
+    <t>48632</t>
+  </si>
+  <si>
+    <t>Controller21564</t>
+  </si>
+  <si>
+    <t>Automation21564</t>
+  </si>
+  <si>
+    <t>controllerautomation21564@gmail.com</t>
+  </si>
+  <si>
+    <t>21564</t>
+  </si>
+  <si>
+    <t>Controller05319</t>
+  </si>
+  <si>
+    <t>Automation05319</t>
+  </si>
+  <si>
+    <t>controllerautomation05319@gmail.com</t>
+  </si>
+  <si>
+    <t>05319</t>
+  </si>
+  <si>
+    <t>Controller56707</t>
+  </si>
+  <si>
+    <t>Automation56707</t>
+  </si>
+  <si>
+    <t>controllerautomation56707@gmail.com</t>
+  </si>
+  <si>
+    <t>56707</t>
+  </si>
+  <si>
+    <t>Controller56972</t>
+  </si>
+  <si>
+    <t>Automation56972</t>
+  </si>
+  <si>
+    <t>controllerautomation56972@gmail.com</t>
+  </si>
+  <si>
+    <t>56972</t>
+  </si>
+  <si>
+    <t>Controller43073</t>
+  </si>
+  <si>
+    <t>Automation43073</t>
+  </si>
+  <si>
+    <t>controllerautomation43073@gmail.com</t>
+  </si>
+  <si>
+    <t>43073</t>
+  </si>
+  <si>
+    <t>Controller46568</t>
+  </si>
+  <si>
+    <t>Automation46568</t>
+  </si>
+  <si>
+    <t>controllerautomation46568@gmail.com</t>
+  </si>
+  <si>
+    <t>46568</t>
+  </si>
+  <si>
+    <t>Controller85190</t>
+  </si>
+  <si>
+    <t>Automation85190</t>
+  </si>
+  <si>
+    <t>controllerautomation85190@gmail.com</t>
+  </si>
+  <si>
+    <t>85190</t>
+  </si>
+  <si>
+    <t>Controller87969</t>
+  </si>
+  <si>
+    <t>Automation87969</t>
+  </si>
+  <si>
+    <t>controllerautomation87969@gmail.com</t>
+  </si>
+  <si>
+    <t>87969</t>
+  </si>
+  <si>
+    <t>Controller05980</t>
+  </si>
+  <si>
+    <t>Automation05980</t>
+  </si>
+  <si>
+    <t>controllerautomation05980@gmail.com</t>
+  </si>
+  <si>
+    <t>05980</t>
+  </si>
+  <si>
+    <t>Controller78554</t>
+  </si>
+  <si>
+    <t>Automation78554</t>
+  </si>
+  <si>
+    <t>controllerautomation78554@gmail.com</t>
+  </si>
+  <si>
+    <t>78554</t>
+  </si>
+  <si>
+    <t>Controller54638</t>
+  </si>
+  <si>
+    <t>Automation54638</t>
+  </si>
+  <si>
+    <t>controllerautomation54638@gmail.com</t>
+  </si>
+  <si>
+    <t>54638</t>
+  </si>
+  <si>
+    <t>Controller00298</t>
+  </si>
+  <si>
+    <t>Automation00298</t>
+  </si>
+  <si>
+    <t>controllerautomation00298@gmail.com</t>
+  </si>
+  <si>
+    <t>00298</t>
+  </si>
+  <si>
+    <t>Controller39555</t>
+  </si>
+  <si>
+    <t>Automation39555</t>
+  </si>
+  <si>
+    <t>controllerautomation39555@gmail.com</t>
+  </si>
+  <si>
+    <t>39555</t>
+  </si>
+  <si>
+    <t>Controller49743</t>
+  </si>
+  <si>
+    <t>Automation49743</t>
+  </si>
+  <si>
+    <t>controllerautomation49743@gmail.com</t>
+  </si>
+  <si>
+    <t>49743</t>
+  </si>
+  <si>
+    <t>Controller37875</t>
+  </si>
+  <si>
+    <t>Automation37875</t>
+  </si>
+  <si>
+    <t>controllerautomation37875@gmail.com</t>
+  </si>
+  <si>
+    <t>37875</t>
+  </si>
+  <si>
+    <t>Controller37949</t>
+  </si>
+  <si>
+    <t>Automation37949</t>
+  </si>
+  <si>
+    <t>controllerautomation37949@gmail.com</t>
+  </si>
+  <si>
+    <t>37949</t>
+  </si>
+  <si>
+    <t>Controller96906</t>
+  </si>
+  <si>
+    <t>Automation96906</t>
+  </si>
+  <si>
+    <t>controllerautomation96906@gmail.com</t>
+  </si>
+  <si>
+    <t>96906</t>
+  </si>
+  <si>
+    <t>Controller95345</t>
+  </si>
+  <si>
+    <t>Automation95345</t>
+  </si>
+  <si>
+    <t>controllerautomation95345@gmail.com</t>
+  </si>
+  <si>
+    <t>95345</t>
+  </si>
+  <si>
+    <t>Controller59951</t>
+  </si>
+  <si>
+    <t>Automation59951</t>
+  </si>
+  <si>
+    <t>controllerautomation59951@gmail.com</t>
+  </si>
+  <si>
+    <t>59951</t>
+  </si>
+  <si>
+    <t>Controller23550</t>
+  </si>
+  <si>
+    <t>Automation23550</t>
+  </si>
+  <si>
+    <t>controllerautomation23550@gmail.com</t>
+  </si>
+  <si>
+    <t>23550</t>
+  </si>
+  <si>
+    <t>Controller62117</t>
+  </si>
+  <si>
+    <t>Automation62117</t>
+  </si>
+  <si>
+    <t>controllerautomation62117@gmail.com</t>
+  </si>
+  <si>
+    <t>62117</t>
+  </si>
+  <si>
+    <t>Controller76233</t>
+  </si>
+  <si>
+    <t>Automation76233</t>
+  </si>
+  <si>
+    <t>controllerautomation76233@gmail.com</t>
+  </si>
+  <si>
+    <t>76233</t>
+  </si>
+  <si>
+    <t>Controller87010</t>
+  </si>
+  <si>
+    <t>Automation87010</t>
+  </si>
+  <si>
+    <t>controllerautomation87010@gmail.com</t>
+  </si>
+  <si>
+    <t>87010</t>
+  </si>
+  <si>
+    <t>Controller02005</t>
+  </si>
+  <si>
+    <t>Automation02005</t>
+  </si>
+  <si>
+    <t>controllerautomation02005@gmail.com</t>
+  </si>
+  <si>
+    <t>02005</t>
+  </si>
+  <si>
+    <t>Controller09283</t>
+  </si>
+  <si>
+    <t>Automation09283</t>
+  </si>
+  <si>
+    <t>controllerautomation09283@gmail.com</t>
+  </si>
+  <si>
+    <t>09283</t>
+  </si>
+  <si>
+    <t>Controller73093</t>
+  </si>
+  <si>
+    <t>Automation73093</t>
+  </si>
+  <si>
+    <t>controllerautomation73093@gmail.com</t>
+  </si>
+  <si>
+    <t>73093</t>
+  </si>
+  <si>
+    <t>Controller60312</t>
+  </si>
+  <si>
+    <t>Automation60312</t>
+  </si>
+  <si>
+    <t>controllerautomation60312@gmail.com</t>
+  </si>
+  <si>
+    <t>60312</t>
+  </si>
+  <si>
+    <t>Controller12988</t>
+  </si>
+  <si>
+    <t>Automation12988</t>
+  </si>
+  <si>
+    <t>controllerautomation12988@gmail.com</t>
+  </si>
+  <si>
+    <t>12988</t>
+  </si>
+  <si>
+    <t>Controller59113</t>
+  </si>
+  <si>
+    <t>Automation59113</t>
+  </si>
+  <si>
+    <t>controllerautomation59113@gmail.com</t>
+  </si>
+  <si>
+    <t>59113</t>
+  </si>
+  <si>
+    <t>Controller28374</t>
+  </si>
+  <si>
+    <t>Automation28374</t>
+  </si>
+  <si>
+    <t>controllerautomation28374@gmail.com</t>
+  </si>
+  <si>
+    <t>28374</t>
+  </si>
+  <si>
+    <t>Controller33572</t>
+  </si>
+  <si>
+    <t>Automation33572</t>
+  </si>
+  <si>
+    <t>controllerautomation33572@gmail.com</t>
+  </si>
+  <si>
+    <t>33572</t>
+  </si>
+  <si>
+    <t>Controller93934</t>
+  </si>
+  <si>
+    <t>Automation93934</t>
+  </si>
+  <si>
+    <t>controllerautomation93934@gmail.com</t>
+  </si>
+  <si>
+    <t>93934</t>
+  </si>
+  <si>
+    <t>Controller29269</t>
+  </si>
+  <si>
+    <t>Automation29269</t>
+  </si>
+  <si>
+    <t>controllerautomation29269@gmail.com</t>
+  </si>
+  <si>
+    <t>29269</t>
+  </si>
+  <si>
+    <t>Controller77009</t>
+  </si>
+  <si>
+    <t>Automation77009</t>
+  </si>
+  <si>
+    <t>controllerautomation77009@gmail.com</t>
+  </si>
+  <si>
+    <t>77009</t>
+  </si>
+  <si>
+    <t>Controller55890</t>
+  </si>
+  <si>
+    <t>Automation55890</t>
+  </si>
+  <si>
+    <t>controllerautomation55890@gmail.com</t>
+  </si>
+  <si>
+    <t>55890</t>
+  </si>
+  <si>
+    <t>Controller00626</t>
+  </si>
+  <si>
+    <t>Automation00626</t>
+  </si>
+  <si>
+    <t>controllerautomation00626@gmail.com</t>
+  </si>
+  <si>
+    <t>00626</t>
+  </si>
+  <si>
+    <t>Controller04009</t>
+  </si>
+  <si>
+    <t>Automation04009</t>
+  </si>
+  <si>
+    <t>controllerautomation04009@gmail.com</t>
+  </si>
+  <si>
+    <t>04009</t>
+  </si>
+  <si>
+    <t>Controller29345</t>
+  </si>
+  <si>
+    <t>Automation29345</t>
+  </si>
+  <si>
+    <t>controllerautomation29345@gmail.com</t>
+  </si>
+  <si>
+    <t>29345</t>
+  </si>
+  <si>
+    <t>Controller08188</t>
+  </si>
+  <si>
+    <t>Automation08188</t>
+  </si>
+  <si>
+    <t>controllerautomation08188@gmail.com</t>
+  </si>
+  <si>
+    <t>08188</t>
+  </si>
+  <si>
+    <t>Controller54993</t>
+  </si>
+  <si>
+    <t>Automation54993</t>
+  </si>
+  <si>
+    <t>controllerautomation54993@gmail.com</t>
+  </si>
+  <si>
+    <t>54993</t>
+  </si>
+  <si>
+    <t>Controller23137</t>
+  </si>
+  <si>
+    <t>Automation23137</t>
+  </si>
+  <si>
+    <t>controllerautomation23137@gmail.com</t>
+  </si>
+  <si>
+    <t>23137</t>
+  </si>
+  <si>
+    <t>Controller72963</t>
+  </si>
+  <si>
+    <t>Automation72963</t>
+  </si>
+  <si>
+    <t>controllerautomation72963@gmail.com</t>
+  </si>
+  <si>
+    <t>72963</t>
+  </si>
+  <si>
+    <t>Controller78770</t>
+  </si>
+  <si>
+    <t>Automation78770</t>
+  </si>
+  <si>
+    <t>controllerautomation78770@gmail.com</t>
+  </si>
+  <si>
+    <t>78770</t>
+  </si>
+  <si>
+    <t>Controller08748</t>
+  </si>
+  <si>
+    <t>Automation08748</t>
+  </si>
+  <si>
+    <t>controllerautomation08748@gmail.com</t>
+  </si>
+  <si>
+    <t>08748</t>
+  </si>
+  <si>
+    <t>Controller57071</t>
+  </si>
+  <si>
+    <t>Automation57071</t>
+  </si>
+  <si>
+    <t>controllerautomation57071@gmail.com</t>
+  </si>
+  <si>
+    <t>57071</t>
+  </si>
+  <si>
+    <t>Controller14426</t>
+  </si>
+  <si>
+    <t>Automation14426</t>
+  </si>
+  <si>
+    <t>controllerautomation14426@gmail.com</t>
+  </si>
+  <si>
+    <t>14426</t>
+  </si>
+  <si>
+    <t>Controller16950</t>
+  </si>
+  <si>
+    <t>Automation16950</t>
+  </si>
+  <si>
+    <t>controllerautomation16950@gmail.com</t>
+  </si>
+  <si>
+    <t>16950</t>
+  </si>
+  <si>
+    <t>Controller44606</t>
+  </si>
+  <si>
+    <t>Automation44606</t>
+  </si>
+  <si>
+    <t>controllerautomation44606@gmail.com</t>
+  </si>
+  <si>
+    <t>44606</t>
+  </si>
+  <si>
+    <t>Controller58914</t>
+  </si>
+  <si>
+    <t>Automation58914</t>
+  </si>
+  <si>
+    <t>controllerautomation58914@gmail.com</t>
+  </si>
+  <si>
+    <t>58914</t>
+  </si>
+  <si>
+    <t>Controller15464</t>
+  </si>
+  <si>
+    <t>Automation15464</t>
+  </si>
+  <si>
+    <t>controllerautomation15464@gmail.com</t>
+  </si>
+  <si>
+    <t>15464</t>
+  </si>
+  <si>
+    <t>Controller46797</t>
+  </si>
+  <si>
+    <t>Automation46797</t>
+  </si>
+  <si>
+    <t>controllerautomation46797@gmail.com</t>
+  </si>
+  <si>
+    <t>46797</t>
+  </si>
+  <si>
+    <t>Controller03220</t>
+  </si>
+  <si>
+    <t>Automation03220</t>
+  </si>
+  <si>
+    <t>controllerautomation03220@gmail.com</t>
+  </si>
+  <si>
+    <t>03220</t>
+  </si>
+  <si>
+    <t>Controller58747</t>
+  </si>
+  <si>
+    <t>Automation58747</t>
+  </si>
+  <si>
+    <t>controllerautomation58747@gmail.com</t>
+  </si>
+  <si>
+    <t>58747</t>
+  </si>
+  <si>
+    <t>Controller46717</t>
+  </si>
+  <si>
+    <t>Automation46717</t>
+  </si>
+  <si>
+    <t>controllerautomation46717@gmail.com</t>
+  </si>
+  <si>
+    <t>46717</t>
+  </si>
+  <si>
+    <t>Controller90040</t>
+  </si>
+  <si>
+    <t>Automation90040</t>
+  </si>
+  <si>
+    <t>controllerautomation90040@gmail.com</t>
+  </si>
+  <si>
+    <t>90040</t>
+  </si>
+  <si>
+    <t>Controller12086</t>
+  </si>
+  <si>
+    <t>Automation12086</t>
+  </si>
+  <si>
+    <t>controllerautomation12086@gmail.com</t>
+  </si>
+  <si>
+    <t>12086</t>
+  </si>
+  <si>
+    <t>Controller89034</t>
+  </si>
+  <si>
+    <t>Automation89034</t>
+  </si>
+  <si>
+    <t>controllerautomation89034@gmail.com</t>
+  </si>
+  <si>
+    <t>89034</t>
+  </si>
+  <si>
+    <t>Controller51162</t>
+  </si>
+  <si>
+    <t>Automation51162</t>
+  </si>
+  <si>
+    <t>controllerautomation51162@gmail.com</t>
+  </si>
+  <si>
+    <t>51162</t>
+  </si>
+  <si>
+    <t>Controller43773</t>
+  </si>
+  <si>
+    <t>Automation43773</t>
+  </si>
+  <si>
+    <t>controllerautomation43773@gmail.com</t>
+  </si>
+  <si>
+    <t>43773</t>
+  </si>
+  <si>
+    <t>Controller38450</t>
+  </si>
+  <si>
+    <t>Automation38450</t>
+  </si>
+  <si>
+    <t>controllerautomation38450@gmail.com</t>
+  </si>
+  <si>
+    <t>38450</t>
+  </si>
+  <si>
+    <t>Controller01015</t>
+  </si>
+  <si>
+    <t>Automation01015</t>
+  </si>
+  <si>
+    <t>controllerautomation01015@gmail.com</t>
+  </si>
+  <si>
+    <t>01015</t>
+  </si>
+  <si>
+    <t>Controller69666</t>
+  </si>
+  <si>
+    <t>Automation69666</t>
+  </si>
+  <si>
+    <t>controllerautomation69666@gmail.com</t>
+  </si>
+  <si>
+    <t>69666</t>
+  </si>
+  <si>
+    <t>Controller50923</t>
+  </si>
+  <si>
+    <t>Automation50923</t>
+  </si>
+  <si>
+    <t>controllerautomation50923@gmail.com</t>
+  </si>
+  <si>
+    <t>50923</t>
+  </si>
+  <si>
+    <t>Controller16187</t>
+  </si>
+  <si>
+    <t>Automation16187</t>
+  </si>
+  <si>
+    <t>controllerautomation16187@gmail.com</t>
+  </si>
+  <si>
+    <t>16187</t>
+  </si>
+  <si>
+    <t>Controller52135</t>
+  </si>
+  <si>
+    <t>Automation52135</t>
+  </si>
+  <si>
+    <t>controllerautomation52135@gmail.com</t>
+  </si>
+  <si>
+    <t>52135</t>
+  </si>
+  <si>
+    <t>Controller15053</t>
+  </si>
+  <si>
+    <t>Automation15053</t>
+  </si>
+  <si>
+    <t>controllerautomation15053@gmail.com</t>
+  </si>
+  <si>
+    <t>15053</t>
+  </si>
+  <si>
+    <t>Controller49369</t>
+  </si>
+  <si>
+    <t>Automation49369</t>
+  </si>
+  <si>
+    <t>controllerautomation49369@gmail.com</t>
+  </si>
+  <si>
+    <t>49369</t>
+  </si>
+  <si>
+    <t>Controller24586</t>
+  </si>
+  <si>
+    <t>Automation24586</t>
+  </si>
+  <si>
+    <t>controllerautomation24586@gmail.com</t>
+  </si>
+  <si>
+    <t>24586</t>
+  </si>
+  <si>
+    <t>Controller54409</t>
+  </si>
+  <si>
+    <t>Automation54409</t>
+  </si>
+  <si>
+    <t>controllerautomation54409@gmail.com</t>
+  </si>
+  <si>
+    <t>54409</t>
+  </si>
+  <si>
+    <t>Controller39598</t>
+  </si>
+  <si>
+    <t>Automation39598</t>
+  </si>
+  <si>
+    <t>controllerautomation39598@gmail.com</t>
+  </si>
+  <si>
+    <t>39598</t>
+  </si>
+  <si>
+    <t>Controller38210</t>
+  </si>
+  <si>
+    <t>Automation38210</t>
+  </si>
+  <si>
+    <t>controllerautomation38210@gmail.com</t>
+  </si>
+  <si>
+    <t>38210</t>
+  </si>
+  <si>
+    <t>Controller66691</t>
+  </si>
+  <si>
+    <t>Automation66691</t>
+  </si>
+  <si>
+    <t>controllerautomation66691@gmail.com</t>
+  </si>
+  <si>
+    <t>66691</t>
+  </si>
+  <si>
+    <t>Controller40877</t>
+  </si>
+  <si>
+    <t>Automation40877</t>
+  </si>
+  <si>
+    <t>controllerautomation40877@gmail.com</t>
+  </si>
+  <si>
+    <t>40877</t>
+  </si>
+  <si>
+    <t>Controller60897</t>
+  </si>
+  <si>
+    <t>Automation60897</t>
+  </si>
+  <si>
+    <t>controllerautomation60897@gmail.com</t>
+  </si>
+  <si>
+    <t>60897</t>
+  </si>
+  <si>
+    <t>Controller42290</t>
+  </si>
+  <si>
+    <t>Automation42290</t>
+  </si>
+  <si>
+    <t>controllerautomation42290@gmail.com</t>
+  </si>
+  <si>
+    <t>42290</t>
+  </si>
+  <si>
+    <t>Controller24882</t>
+  </si>
+  <si>
+    <t>Automation24882</t>
+  </si>
+  <si>
+    <t>controllerautomation24882@gmail.com</t>
+  </si>
+  <si>
+    <t>24882</t>
+  </si>
+  <si>
+    <t>Controller25854</t>
+  </si>
+  <si>
+    <t>Automation25854</t>
+  </si>
+  <si>
+    <t>controllerautomation25854@gmail.com</t>
+  </si>
+  <si>
+    <t>25854</t>
+  </si>
+  <si>
+    <t>Controller17074</t>
+  </si>
+  <si>
+    <t>Automation17074</t>
+  </si>
+  <si>
+    <t>controllerautomation17074@gmail.com</t>
+  </si>
+  <si>
+    <t>17074</t>
+  </si>
+  <si>
+    <t>Controller73893</t>
+  </si>
+  <si>
+    <t>Automation73893</t>
+  </si>
+  <si>
+    <t>controllerautomation73893@gmail.com</t>
+  </si>
+  <si>
+    <t>73893</t>
+  </si>
+  <si>
+    <t>Controller92758</t>
+  </si>
+  <si>
+    <t>Automation92758</t>
+  </si>
+  <si>
+    <t>controllerautomation92758@gmail.com</t>
+  </si>
+  <si>
+    <t>92758</t>
+  </si>
+  <si>
+    <t>Controller21767</t>
+  </si>
+  <si>
+    <t>Automation21767</t>
+  </si>
+  <si>
+    <t>controllerautomation21767@gmail.com</t>
+  </si>
+  <si>
+    <t>21767</t>
+  </si>
+  <si>
+    <t>Controller39187</t>
+  </si>
+  <si>
+    <t>Automation39187</t>
+  </si>
+  <si>
+    <t>controllerautomation39187@gmail.com</t>
+  </si>
+  <si>
+    <t>39187</t>
+  </si>
+  <si>
+    <t>Controller20694</t>
+  </si>
+  <si>
+    <t>Automation20694</t>
+  </si>
+  <si>
+    <t>controllerautomation20694@gmail.com</t>
+  </si>
+  <si>
+    <t>20694</t>
+  </si>
+  <si>
+    <t>Controller79201</t>
+  </si>
+  <si>
+    <t>Automation79201</t>
+  </si>
+  <si>
+    <t>controllerautomation79201@gmail.com</t>
+  </si>
+  <si>
+    <t>79201</t>
+  </si>
+  <si>
+    <t>Controller26405</t>
+  </si>
+  <si>
+    <t>Automation26405</t>
+  </si>
+  <si>
+    <t>controllerautomation26405@gmail.com</t>
+  </si>
+  <si>
+    <t>26405</t>
+  </si>
+  <si>
+    <t>Controller76231</t>
+  </si>
+  <si>
+    <t>Automation76231</t>
+  </si>
+  <si>
+    <t>controllerautomation76231@gmail.com</t>
+  </si>
+  <si>
+    <t>76231</t>
+  </si>
+  <si>
+    <t>Controller53295</t>
+  </si>
+  <si>
+    <t>Automation53295</t>
+  </si>
+  <si>
+    <t>controllerautomation53295@gmail.com</t>
+  </si>
+  <si>
+    <t>53295</t>
+  </si>
+  <si>
+    <t>Controller22846</t>
+  </si>
+  <si>
+    <t>Automation22846</t>
+  </si>
+  <si>
+    <t>controllerautomation22846@gmail.com</t>
+  </si>
+  <si>
+    <t>22846</t>
   </si>
 </sst>
 </file>
@@ -4535,422 +6323,422 @@
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>1245</v>
+        <v>1845</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>1246</v>
+        <v>1846</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>1247</v>
+        <v>1847</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>1248</v>
+        <v>1848</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>1249</v>
+        <v>1849</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>1250</v>
+        <v>1850</v>
       </c>
       <c r="C3" t="s" s="0">
-        <v>1251</v>
+        <v>1851</v>
       </c>
       <c r="D3" t="s" s="0">
-        <v>1252</v>
+        <v>1852</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>1253</v>
+        <v>1853</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>1254</v>
+        <v>1854</v>
       </c>
       <c r="C4" t="s" s="0">
-        <v>1255</v>
+        <v>1855</v>
       </c>
       <c r="D4" t="s" s="0">
-        <v>1256</v>
+        <v>1856</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>1257</v>
+        <v>1857</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>1258</v>
+        <v>1858</v>
       </c>
       <c r="C5" t="s" s="0">
-        <v>1259</v>
+        <v>1859</v>
       </c>
       <c r="D5" t="s" s="0">
-        <v>1260</v>
+        <v>1860</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>1261</v>
+        <v>1861</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>1262</v>
+        <v>1862</v>
       </c>
       <c r="C6" t="s" s="0">
-        <v>1263</v>
+        <v>1863</v>
       </c>
       <c r="D6" t="s" s="0">
-        <v>1264</v>
+        <v>1864</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>1265</v>
+        <v>1865</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>1266</v>
+        <v>1866</v>
       </c>
       <c r="C7" t="s" s="0">
-        <v>1267</v>
+        <v>1867</v>
       </c>
       <c r="D7" t="s" s="0">
-        <v>1268</v>
+        <v>1868</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>1269</v>
+        <v>1869</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>1270</v>
+        <v>1870</v>
       </c>
       <c r="C8" t="s" s="0">
-        <v>1271</v>
+        <v>1871</v>
       </c>
       <c r="D8" t="s" s="0">
-        <v>1272</v>
+        <v>1872</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>1273</v>
+        <v>1873</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>1274</v>
+        <v>1874</v>
       </c>
       <c r="C9" t="s" s="0">
-        <v>1275</v>
+        <v>1875</v>
       </c>
       <c r="D9" t="s" s="0">
-        <v>1276</v>
+        <v>1876</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>1277</v>
+        <v>1877</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>1278</v>
+        <v>1878</v>
       </c>
       <c r="C10" t="s" s="0">
-        <v>1279</v>
+        <v>1879</v>
       </c>
       <c r="D10" t="s" s="0">
-        <v>1280</v>
+        <v>1880</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>1281</v>
+        <v>741</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>1282</v>
+        <v>742</v>
       </c>
       <c r="C11" t="s" s="0">
-        <v>1283</v>
+        <v>743</v>
       </c>
       <c r="D11" t="s" s="0">
-        <v>1284</v>
+        <v>744</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>1285</v>
+        <v>1881</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>1286</v>
+        <v>1882</v>
       </c>
       <c r="C12" t="s" s="0">
-        <v>1287</v>
+        <v>1883</v>
       </c>
       <c r="D12" t="s" s="0">
-        <v>1288</v>
+        <v>1884</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>1289</v>
+        <v>1885</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>1290</v>
+        <v>1886</v>
       </c>
       <c r="C13" t="s" s="0">
-        <v>1291</v>
+        <v>1887</v>
       </c>
       <c r="D13" t="s" s="0">
-        <v>1292</v>
+        <v>1888</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>1293</v>
+        <v>1889</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>1294</v>
+        <v>1890</v>
       </c>
       <c r="C14" t="s" s="0">
-        <v>1295</v>
+        <v>1891</v>
       </c>
       <c r="D14" t="s" s="0">
-        <v>1296</v>
+        <v>1892</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>1297</v>
+        <v>1893</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>1298</v>
+        <v>1894</v>
       </c>
       <c r="C15" t="s" s="0">
-        <v>1299</v>
+        <v>1895</v>
       </c>
       <c r="D15" t="s" s="0">
-        <v>1300</v>
+        <v>1896</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>1301</v>
+        <v>1897</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>1302</v>
+        <v>1898</v>
       </c>
       <c r="C16" t="s" s="0">
-        <v>1303</v>
+        <v>1899</v>
       </c>
       <c r="D16" t="s" s="0">
-        <v>1304</v>
+        <v>1900</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>1305</v>
+        <v>1901</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>1306</v>
+        <v>1902</v>
       </c>
       <c r="C17" t="s" s="0">
-        <v>1307</v>
+        <v>1903</v>
       </c>
       <c r="D17" t="s" s="0">
-        <v>1308</v>
+        <v>1904</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>1309</v>
+        <v>1905</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>1310</v>
+        <v>1906</v>
       </c>
       <c r="C18" t="s" s="0">
-        <v>1311</v>
+        <v>1907</v>
       </c>
       <c r="D18" t="s" s="0">
-        <v>1312</v>
+        <v>1908</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>1313</v>
+        <v>1909</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>1314</v>
+        <v>1910</v>
       </c>
       <c r="C19" t="s" s="0">
-        <v>1315</v>
+        <v>1911</v>
       </c>
       <c r="D19" t="s" s="0">
-        <v>1316</v>
+        <v>1912</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>1317</v>
+        <v>1913</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>1318</v>
+        <v>1914</v>
       </c>
       <c r="C20" t="s" s="0">
-        <v>1319</v>
+        <v>1915</v>
       </c>
       <c r="D20" t="s" s="0">
-        <v>1320</v>
+        <v>1916</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>1321</v>
+        <v>1917</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>1322</v>
+        <v>1918</v>
       </c>
       <c r="C21" t="s" s="0">
-        <v>1323</v>
+        <v>1919</v>
       </c>
       <c r="D21" t="s" s="0">
-        <v>1324</v>
+        <v>1920</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>1325</v>
+        <v>1921</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>1326</v>
+        <v>1922</v>
       </c>
       <c r="C22" t="s" s="0">
-        <v>1327</v>
+        <v>1923</v>
       </c>
       <c r="D22" t="s" s="0">
-        <v>1328</v>
+        <v>1924</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
-        <v>1329</v>
+        <v>1925</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>1330</v>
+        <v>1926</v>
       </c>
       <c r="C23" t="s" s="0">
-        <v>1331</v>
+        <v>1927</v>
       </c>
       <c r="D23" t="s" s="0">
-        <v>1332</v>
+        <v>1928</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="0">
-        <v>1333</v>
+        <v>1929</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>1334</v>
+        <v>1930</v>
       </c>
       <c r="C24" t="s" s="0">
-        <v>1335</v>
+        <v>1931</v>
       </c>
       <c r="D24" t="s" s="0">
-        <v>1336</v>
+        <v>1932</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="0">
-        <v>1337</v>
+        <v>1933</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>1338</v>
+        <v>1934</v>
       </c>
       <c r="C25" t="s" s="0">
-        <v>1339</v>
+        <v>1935</v>
       </c>
       <c r="D25" t="s" s="0">
-        <v>1340</v>
+        <v>1936</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="0">
-        <v>1341</v>
+        <v>1937</v>
       </c>
       <c r="B26" t="s" s="0">
-        <v>1342</v>
+        <v>1938</v>
       </c>
       <c r="C26" t="s" s="0">
-        <v>1343</v>
+        <v>1939</v>
       </c>
       <c r="D26" t="s" s="0">
-        <v>1344</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="0">
-        <v>1345</v>
+        <v>1941</v>
       </c>
       <c r="B27" t="s" s="0">
-        <v>1346</v>
+        <v>1942</v>
       </c>
       <c r="C27" t="s" s="0">
-        <v>1347</v>
+        <v>1943</v>
       </c>
       <c r="D27" t="s" s="0">
-        <v>1348</v>
+        <v>1944</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s" s="0">
-        <v>1349</v>
+        <v>1945</v>
       </c>
       <c r="B28" t="s" s="0">
-        <v>1350</v>
+        <v>1946</v>
       </c>
       <c r="C28" t="s" s="0">
-        <v>1351</v>
+        <v>1947</v>
       </c>
       <c r="D28" t="s" s="0">
-        <v>1352</v>
+        <v>1948</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s" s="0">
-        <v>1353</v>
+        <v>1949</v>
       </c>
       <c r="B29" t="s" s="0">
-        <v>1354</v>
+        <v>1950</v>
       </c>
       <c r="C29" t="s" s="0">
-        <v>1355</v>
+        <v>1951</v>
       </c>
       <c r="D29" t="s" s="0">
-        <v>1356</v>
+        <v>1952</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s" s="0">
-        <v>1357</v>
+        <v>1953</v>
       </c>
       <c r="B30" t="s" s="0">
-        <v>1358</v>
+        <v>1954</v>
       </c>
       <c r="C30" t="s" s="0">
-        <v>1359</v>
+        <v>1955</v>
       </c>
       <c r="D30" t="s" s="0">
-        <v>1360</v>
+        <v>1956</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s" s="0">
-        <v>1361</v>
+        <v>1957</v>
       </c>
       <c r="B31" t="s" s="0">
-        <v>1362</v>
+        <v>1958</v>
       </c>
       <c r="C31" t="s" s="0">
-        <v>1363</v>
+        <v>1959</v>
       </c>
       <c r="D31" t="s" s="0">
-        <v>1364</v>
+        <v>1960</v>
       </c>
     </row>
   </sheetData>

</xml_diff>